<commit_message>
set zustand to manage controller states
</commit_message>
<xml_diff>
--- a/components/PortalXR/buttonConfiguration.xlsx
+++ b/components/PortalXR/buttonConfiguration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/portal301/workspace/nextjs-portal301/components/PortalXR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35ECA31-3A95-3C43-A21C-03576C52158E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E69D6EB-8758-6948-8B56-29D984E9EC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="18200" windowHeight="14000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32640" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plan" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
   <si>
     <t>RIGHT</t>
   </si>
@@ -116,6 +116,10 @@
   <si>
     <t>spatial video z position(앞뒤) 
 / y rotation</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>controller mode</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -204,44 +208,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,14 +554,17 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="8.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5" style="8" bestFit="1" customWidth="1"/>
@@ -566,21 +573,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="9"/>
-      <c r="B1" s="10"/>
-      <c r="D1" s="11" t="s">
+      <c r="A1" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="16" t="s">
@@ -588,205 +598,205 @@
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="16"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:10" ht="33">
       <c r="A4" s="16"/>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="16"/>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10" ht="33">
       <c r="A6" s="16"/>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11" t="s">
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="16"/>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="16"/>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>5</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>0</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="16"/>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <v>1</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" ht="49">
       <c r="A11" s="16"/>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>2</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11" t="s">
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="49">
       <c r="A12" s="16"/>
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <v>3</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11" t="s">
+      <c r="D12" s="10"/>
+      <c r="E12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" s="13" customFormat="1">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" s="12" customFormat="1">
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="16" t="s">
@@ -794,180 +804,181 @@
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="16"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <v>0</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="16"/>
-      <c r="B16" s="10">
+      <c r="B16" s="9">
         <v>1</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="16"/>
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <v>2</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="16"/>
-      <c r="B18" s="10">
+      <c r="B18" s="9">
         <v>3</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="16"/>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>4</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="16"/>
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <v>5</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <v>0</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="16"/>
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <v>1</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="16"/>
-      <c r="B23" s="10">
+      <c r="B23" s="9">
         <v>2</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="16"/>
-      <c r="B24" s="10">
+      <c r="B24" s="9">
         <v>3</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:A8"/>
@@ -1016,7 +1027,7 @@
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="18" customHeight="1">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2">
@@ -1124,7 +1135,7 @@
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="18" customHeight="1">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="18" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="2">
@@ -1230,7 +1241,7 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="2">
@@ -1328,7 +1339,7 @@
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" ht="18" customHeight="1">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="18" t="s">
         <v>13</v>
       </c>
       <c r="B22" s="2">

</xml_diff>

<commit_message>
adding XR UI.. not completed..
</commit_message>
<xml_diff>
--- a/components/PortalXR/buttonConfiguration.xlsx
+++ b/components/PortalXR/buttonConfiguration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/portal301/workspace/nextjs-portal301/components/PortalXR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E69D6EB-8758-6948-8B56-29D984E9EC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D378884D-AF41-A247-82DD-8A717310BBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32640" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32640" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plan" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
   <si>
     <t>RIGHT</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>switch mode</t>
-  </si>
-  <si>
-    <t>gripper control?</t>
   </si>
   <si>
     <t>spatial video x position(좌우) 
@@ -120,6 +117,18 @@
   </si>
   <si>
     <t>controller mode</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>select</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>gripper control</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>align short key</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -227,6 +236,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -243,9 +255,6 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,7 +567,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -573,11 +582,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="A1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
       <c r="D1" s="10" t="s">
         <v>22</v>
       </c>
@@ -593,11 +602,11 @@
       <c r="J1" s="10"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="16"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -607,7 +616,7 @@
       <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="9">
@@ -622,14 +631,16 @@
       <c r="E3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="10"/>
+      <c r="F3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:10" ht="33">
-      <c r="A4" s="16"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="9">
         <v>1</v>
       </c>
@@ -647,7 +658,7 @@
       <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="16"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="9">
         <v>2</v>
       </c>
@@ -663,7 +674,7 @@
       <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10" ht="33">
-      <c r="A6" s="16"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="9">
         <v>3</v>
       </c>
@@ -681,7 +692,7 @@
       <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="16"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="9">
         <v>4</v>
       </c>
@@ -689,7 +700,9 @@
         <v>9</v>
       </c>
       <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -697,7 +710,7 @@
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="16"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="9">
         <v>5</v>
       </c>
@@ -707,15 +720,19 @@
       <c r="D8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="9">
@@ -733,7 +750,7 @@
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="16"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="9">
         <v>1</v>
       </c>
@@ -749,7 +766,7 @@
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" ht="49">
-      <c r="A11" s="16"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="9">
         <v>2</v>
       </c>
@@ -759,7 +776,7 @@
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -767,7 +784,7 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="49">
-      <c r="A12" s="16"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="9">
         <v>3</v>
       </c>
@@ -776,10 +793,10 @@
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>29</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -799,11 +816,11 @@
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="16"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -813,7 +830,7 @@
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="9">
@@ -831,7 +848,7 @@
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="16"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="9">
         <v>1</v>
       </c>
@@ -847,7 +864,7 @@
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="16"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="9">
         <v>2</v>
       </c>
@@ -863,7 +880,7 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="16"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="9">
         <v>3</v>
       </c>
@@ -879,7 +896,7 @@
       <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="16"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="9">
         <v>4</v>
       </c>
@@ -895,7 +912,7 @@
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="16"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="9">
         <v>5</v>
       </c>
@@ -911,7 +928,7 @@
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="9">
@@ -929,7 +946,7 @@
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="16"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="9">
         <v>1</v>
       </c>
@@ -945,7 +962,7 @@
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="16"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="9">
         <v>2</v>
       </c>
@@ -961,7 +978,7 @@
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="16"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="9">
         <v>3</v>
       </c>
@@ -1018,16 +1035,16 @@
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="19"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="20"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="18" customHeight="1">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2">
@@ -1047,7 +1064,7 @@
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="18" customHeight="1">
-      <c r="A4" s="19"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -1065,7 +1082,7 @@
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" ht="18" customHeight="1">
-      <c r="A5" s="19"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -1081,7 +1098,7 @@
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" ht="18" customHeight="1">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="2">
         <v>3</v>
       </c>
@@ -1099,7 +1116,7 @@
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="18" customHeight="1">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="2">
         <v>4</v>
       </c>
@@ -1117,7 +1134,7 @@
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="18" customHeight="1">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="2">
         <v>5</v>
       </c>
@@ -1135,7 +1152,7 @@
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="18" customHeight="1">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="19" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="2">
@@ -1153,7 +1170,7 @@
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" ht="18" customHeight="1">
-      <c r="A10" s="19"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="2">
         <v>1</v>
       </c>
@@ -1169,7 +1186,7 @@
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="2">
         <v>2</v>
       </c>
@@ -1187,7 +1204,7 @@
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="18" customHeight="1">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="2">
         <v>3</v>
       </c>
@@ -1227,11 +1244,11 @@
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" ht="18" customHeight="1">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="19"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -1241,7 +1258,7 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="2">
@@ -1259,7 +1276,7 @@
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="18" customHeight="1">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="2">
         <v>1</v>
       </c>
@@ -1275,7 +1292,7 @@
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="18" customHeight="1">
-      <c r="A18" s="19"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="2">
         <v>2</v>
       </c>
@@ -1291,7 +1308,7 @@
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" ht="18" customHeight="1">
-      <c r="A19" s="19"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="2">
         <v>3</v>
       </c>
@@ -1307,7 +1324,7 @@
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:10" ht="18" customHeight="1">
-      <c r="A20" s="19"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="2">
         <v>4</v>
       </c>
@@ -1323,7 +1340,7 @@
       <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:10" ht="18" customHeight="1">
-      <c r="A21" s="19"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="2">
         <v>5</v>
       </c>
@@ -1339,7 +1356,7 @@
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" ht="18" customHeight="1">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="19" t="s">
         <v>13</v>
       </c>
       <c r="B22" s="2">
@@ -1357,7 +1374,7 @@
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" ht="18" customHeight="1">
-      <c r="A23" s="19"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="2">
         <v>1</v>
       </c>
@@ -1373,7 +1390,7 @@
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:10" ht="18" customHeight="1">
-      <c r="A24" s="19"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="2">
         <v>2</v>
       </c>
@@ -1391,7 +1408,7 @@
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:10" ht="18" customHeight="1">
-      <c r="A25" s="19"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="2">
         <v>3</v>
       </c>

</xml_diff>